<commit_message>
updated model of database
</commit_message>
<xml_diff>
--- a/Documents/model.xlsx
+++ b/Documents/model.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C1824227\Desktop\client_project-group_2\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C65BBFC-C02E-4C1B-A7B1-2EF0BA2A4A4C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA42C6D-0B57-4D97-A01E-2AD8637055E1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{83BA0F28-02DD-486B-AE82-63A92757738F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tip Reports" sheetId="1" r:id="rId1"/>
-    <sheet name="Paths" sheetId="4" r:id="rId2"/>
-    <sheet name="Waste" sheetId="2" r:id="rId3"/>
-    <sheet name="Waste Size" sheetId="3" r:id="rId4"/>
+    <sheet name="Witness" sheetId="6" r:id="rId2"/>
+    <sheet name="Image" sheetId="4" r:id="rId3"/>
+    <sheet name="Waste" sheetId="2" r:id="rId4"/>
+    <sheet name="Waste Size" sheetId="3" r:id="rId5"/>
+    <sheet name="Images" sheetId="5" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Report ID</t>
   </si>
@@ -84,26 +86,85 @@
     <t>Waste Size ID</t>
   </si>
   <si>
+    <t>/uploads/img1</t>
+  </si>
+  <si>
+    <t>Imageid</t>
+  </si>
+  <si>
     <t>pathid</t>
   </si>
   <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>/uploads/img1</t>
-  </si>
-  <si>
-    <t>Pathid</t>
+    <t>imageid</t>
+  </si>
+  <si>
+    <t>/uploads/img2</t>
+  </si>
+  <si>
+    <t>imagepath1</t>
+  </si>
+  <si>
+    <t>imagepath2</t>
+  </si>
+  <si>
+    <t>imagepath3</t>
+  </si>
+  <si>
+    <t>imagepath4</t>
+  </si>
+  <si>
+    <t>witness</t>
+  </si>
+  <si>
+    <t>yes/no</t>
+  </si>
+  <si>
+    <t>witnessid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>Contact number</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Jone</t>
+  </si>
+  <si>
+    <t>emailaddress</t>
+  </si>
+  <si>
+    <t>ben@gamil.com</t>
+  </si>
+  <si>
+    <t>wastedescription</t>
+  </si>
+  <si>
+    <t>optional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,13 +187,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68D7FF-DC29-4E95-AFB4-400B8AE212DC}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,7 +525,7 @@
     <col min="6" max="6" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,10 +542,22 @@
         <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -499,6 +575,67 @@
       </c>
       <c r="F2">
         <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{DF4878B8-CDDF-4A6B-A004-3CF62471DCA9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0F8F0A-6FFA-4728-864F-4368B7329F60}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>7656465746</v>
       </c>
     </row>
   </sheetData>
@@ -506,43 +643,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFFD68EC-1F43-49A9-89AE-A0801CF475DE}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -553,7 +702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71642ACA-E586-4F98-B8C1-B6F741EC7DF7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -603,7 +752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C2CAA3-2915-4130-92C4-9710F4D7E7EE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -648,4 +797,50 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F768FF74-6EED-4336-95EE-553111103DCA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>